<commit_message>
added more dater to the downloaded sheet and also improved upload processing to get new signups working
</commit_message>
<xml_diff>
--- a/server/prasignups6-7-2015.xlsx
+++ b/server/prasignups6-7-2015.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,12 @@
     <t>parseId</t>
   </si>
   <si>
+    <t>jobId</t>
+  </si>
+  <si>
+    <t>eventDate</t>
+  </si>
+  <si>
     <t>Bill McMahon</t>
   </si>
   <si>
@@ -52,6 +58,9 @@
     <t>QHi2lq4KBL</t>
   </si>
   <si>
+    <t>k9uvUH8d1h</t>
+  </si>
+  <si>
     <t>Dan Stone</t>
   </si>
   <si>
@@ -61,6 +70,9 @@
     <t>WTbz16rPW5</t>
   </si>
   <si>
+    <t>Citj7FmHb8</t>
+  </si>
+  <si>
     <t>Deb Carlson</t>
   </si>
   <si>
@@ -70,6 +82,9 @@
     <t>ZP9ocsjsIC</t>
   </si>
   <si>
+    <t>UdTtx4BXbQ</t>
+  </si>
+  <si>
     <t>Sheryl Ladelfa</t>
   </si>
   <si>
@@ -79,15 +94,33 @@
     <t>1iTdfymxJS</t>
   </si>
   <si>
+    <t>yp6lo0WuVh</t>
+  </si>
+  <si>
     <t>Sign-Up/Scoring</t>
   </si>
   <si>
+    <t>G1tr5WEaFN</t>
+  </si>
+  <si>
+    <t>hbgRXiVmfC</t>
+  </si>
+  <si>
+    <t>klWQUZ2aQM</t>
+  </si>
+  <si>
     <t>Sign-Up/Tower Help</t>
   </si>
   <si>
+    <t>czd5FSdZhg</t>
+  </si>
+  <si>
     <t>Front Gate Help/Start Gate</t>
   </si>
   <si>
+    <t>wdevpYXEOR</t>
+  </si>
+  <si>
     <t>Gary Walker</t>
   </si>
   <si>
@@ -97,18 +130,33 @@
     <t>w7M0d4CTkP</t>
   </si>
   <si>
+    <t>QHpKgN0UyI</t>
+  </si>
+  <si>
     <t>Finish Line Flagger</t>
   </si>
   <si>
+    <t>7ZxPeHFeIF</t>
+  </si>
+  <si>
     <t>Mini Track Scoring/Tower Help/Trophy Duty</t>
   </si>
   <si>
+    <t>0YkwV7rS52</t>
+  </si>
+  <si>
     <t>Dist sign-up/Head Scorer</t>
   </si>
   <si>
+    <t>U5gWYyruqM</t>
+  </si>
+  <si>
     <t>Mini Track Scoring</t>
   </si>
   <si>
+    <t>S83g9ViAsQ</t>
+  </si>
+  <si>
     <t>Kevin Piccola</t>
   </si>
   <si>
@@ -118,9 +166,15 @@
     <t>LmUMbmZ2sf</t>
   </si>
   <si>
+    <t>MZMXgMr9pU</t>
+  </si>
+  <si>
     <t>Mini Track -Finish Line flagger/start gate</t>
   </si>
   <si>
+    <t>9Oa0NXLSYw</t>
+  </si>
+  <si>
     <t>Adam swanson</t>
   </si>
   <si>
@@ -130,18 +184,36 @@
     <t>Pe4lafOsE9</t>
   </si>
   <si>
+    <t>uhxIaZmlYl</t>
+  </si>
+  <si>
+    <t>fQslfbVn0Q</t>
+  </si>
+  <si>
+    <t>rlgFbwV61E</t>
+  </si>
+  <si>
     <t>Front/Back Gate 7-3</t>
   </si>
   <si>
+    <t>UJMFPHOX3c</t>
+  </si>
+  <si>
     <t>Front/Back Gate 7-9</t>
   </si>
   <si>
     <t>DR60OsMNNB</t>
   </si>
   <si>
+    <t>9wFrbztqua</t>
+  </si>
+  <si>
     <t>Front Gate 7-12</t>
   </si>
   <si>
+    <t>jqX1P5aAI2</t>
+  </si>
+  <si>
     <t>John Stein</t>
   </si>
   <si>
@@ -151,18 +223,99 @@
     <t>ZArnt6S7Yu</t>
   </si>
   <si>
+    <t>H9ws2Dij5N</t>
+  </si>
+  <si>
     <t>Flagger</t>
   </si>
   <si>
+    <t>APLq4wsfYB</t>
+  </si>
+  <si>
+    <t>Mxot6aGzhc</t>
+  </si>
+  <si>
+    <t>Up4uSbIuFa</t>
+  </si>
+  <si>
+    <t>LevhnCmBKy</t>
+  </si>
+  <si>
+    <t>MK7cxb0smB</t>
+  </si>
+  <si>
+    <t>FXsjsbZh8Y</t>
+  </si>
+  <si>
+    <t>dJPWRH4ZQ5</t>
+  </si>
+  <si>
+    <t>rmnezD4USo</t>
+  </si>
+  <si>
+    <t>PYA5ae0vUz</t>
+  </si>
+  <si>
+    <t>6OTgcgmo7x</t>
+  </si>
+  <si>
+    <t>BUdHDzn8s7</t>
+  </si>
+  <si>
+    <t>yv72N3pjhs</t>
+  </si>
+  <si>
+    <t>UhxiBQGnXt</t>
+  </si>
+  <si>
+    <t>zk5wWEbh4m</t>
+  </si>
+  <si>
+    <t>xqZcyWX3g2</t>
+  </si>
+  <si>
     <t>Track Maintenance/Relief Flagger</t>
   </si>
   <si>
+    <t>8e3ZNf8EQo</t>
+  </si>
+  <si>
+    <t>Faa31l8bLx</t>
+  </si>
+  <si>
+    <t>3FN4ojYXko</t>
+  </si>
+  <si>
+    <t>Ahrmge5hqH</t>
+  </si>
+  <si>
+    <t>3YufvBR0YO</t>
+  </si>
+  <si>
+    <t>F9js6vpTHk</t>
+  </si>
+  <si>
     <t>Facility Clean up</t>
   </si>
   <si>
+    <t>SG0wWOMpJE</t>
+  </si>
+  <si>
+    <t>MVEwkM1EPj</t>
+  </si>
+  <si>
+    <t>YfCHefhPOC</t>
+  </si>
+  <si>
+    <t>525W4PaEvC</t>
+  </si>
+  <si>
     <t>Bathroom Maintenance</t>
   </si>
   <si>
+    <t>W0VlLpJxBS</t>
+  </si>
+  <si>
     <t>Lyons Ambulance</t>
   </si>
   <si>
@@ -172,12 +325,21 @@
     <t>6s8hGoHKzR</t>
   </si>
   <si>
+    <t>HHWHQKJ2eO</t>
+  </si>
+  <si>
     <t>Announcer</t>
   </si>
   <si>
+    <t>qiNIMAoeUo</t>
+  </si>
+  <si>
     <t>WNY Racing Ref</t>
   </si>
   <si>
+    <t>aIvH8s8Nfe</t>
+  </si>
+  <si>
     <t>brain Wolfe</t>
   </si>
   <si>
@@ -187,15 +349,24 @@
     <t>S8BGd6jwGK</t>
   </si>
   <si>
+    <t>q8LmOBQuHs</t>
+  </si>
+  <si>
     <t>annette wolfe</t>
   </si>
   <si>
     <t>Ah2qy4mN01</t>
   </si>
   <si>
+    <t>3CYpi1Ixk4</t>
+  </si>
+  <si>
     <t>Sat. Front gate 7-11</t>
   </si>
   <si>
+    <t>akz8tOv0e5</t>
+  </si>
+  <si>
     <t>Michele Jones</t>
   </si>
   <si>
@@ -205,6 +376,9 @@
     <t>61B3okH6fG</t>
   </si>
   <si>
+    <t>9k3lUOnlXJ</t>
+  </si>
+  <si>
     <t>brian wolfe</t>
   </si>
   <si>
@@ -214,6 +388,12 @@
     <t>tY5JWcj5Fa</t>
   </si>
   <si>
+    <t>xvUj1j8g3z</t>
+  </si>
+  <si>
+    <t>dnaqC7IBvz</t>
+  </si>
+  <si>
     <t>Alan Delimon</t>
   </si>
   <si>
@@ -223,13 +403,76 @@
     <t>CZX3Ddms0e</t>
   </si>
   <si>
+    <t>PoJOD5hr4c</t>
+  </si>
+  <si>
     <t>EkfyEgvOt4</t>
   </si>
   <si>
+    <t>9JhALBFIlN</t>
+  </si>
+  <si>
+    <t>VkpJv5WQVK</t>
+  </si>
+  <si>
+    <t>8EiJ2bEgxS</t>
+  </si>
+  <si>
+    <t>8gxG5mA9pn</t>
+  </si>
+  <si>
+    <t>940fZLQ8Wp</t>
+  </si>
+  <si>
+    <t>xPSiJQLYWy</t>
+  </si>
+  <si>
+    <t>lnLXNHWJiJ</t>
+  </si>
+  <si>
+    <t>Y8g9fqvK5M</t>
+  </si>
+  <si>
+    <t>AzLEzsVkhL</t>
+  </si>
+  <si>
     <t>Friday Night Watering</t>
   </si>
   <si>
     <t>qafgF1hIO1</t>
+  </si>
+  <si>
+    <t>k2zs7OHk1E</t>
+  </si>
+  <si>
+    <t>0fKUAUtyfO</t>
+  </si>
+  <si>
+    <t>WVO2mNwo4b</t>
+  </si>
+  <si>
+    <t>CXMUuim1AY</t>
+  </si>
+  <si>
+    <t>Ozd2Qhc9jh</t>
+  </si>
+  <si>
+    <t>iTUJACaPTn</t>
+  </si>
+  <si>
+    <t>JLBnCS8NVM</t>
+  </si>
+  <si>
+    <t>JNqQFLj7S1</t>
+  </si>
+  <si>
+    <t>OawwiG0RAD</t>
+  </si>
+  <si>
+    <t>F6nWwTtDMU</t>
+  </si>
+  <si>
+    <t>6-7-2015</t>
   </si>
 </sst>
 </file>
@@ -793,7 +1036,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -806,9 +1049,11 @@
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
     <col min="7" max="7" width="0" customWidth="1"/>
+    <col min="8" max="8" width="0" customWidth="1"/>
+    <col min="9" max="9" width="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -830,13 +1075,19 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3">
         <v>3</v>
@@ -845,21 +1096,24 @@
         <v>0</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5">
         <v>3</v>
@@ -868,21 +1122,24 @@
         <v>0</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="3">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -891,21 +1148,24 @@
         <v>0</v>
       </c>
       <c r="E4" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s" s="3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="5">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5">
         <v>3</v>
@@ -914,21 +1174,24 @@
         <v>0</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <v>3</v>
@@ -937,21 +1200,24 @@
         <v>125</v>
       </c>
       <c r="E6" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5">
         <v>3</v>
@@ -960,21 +1226,24 @@
         <v>125</v>
       </c>
       <c r="E7" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3">
         <v>3</v>
@@ -983,21 +1252,24 @@
         <v>125</v>
       </c>
       <c r="E8" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C9" s="5">
         <v>3</v>
@@ -1006,21 +1278,24 @@
         <v>125</v>
       </c>
       <c r="E9" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3">
         <v>3</v>
@@ -1029,21 +1304,24 @@
         <v>125</v>
       </c>
       <c r="E10" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s" s="5">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
@@ -1052,21 +1330,24 @@
         <v>125</v>
       </c>
       <c r="E11" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s" s="5">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3">
         <v>3</v>
@@ -1075,21 +1356,24 @@
         <v>125</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
@@ -1098,21 +1382,24 @@
         <v>125</v>
       </c>
       <c r="E13" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C14" s="3">
         <v>3</v>
@@ -1121,21 +1408,24 @@
         <v>125</v>
       </c>
       <c r="E14" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s" s="18">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C15" s="18">
         <v>1</v>
@@ -1144,21 +1434,24 @@
         <v>0</v>
       </c>
       <c r="E15" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s" s="18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s" s="20">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s" s="20">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C16" s="20">
         <v>2</v>
@@ -1167,21 +1460,24 @@
         <v>30</v>
       </c>
       <c r="E16" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s" s="20">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="H16" t="s" s="20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s" s="18">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C17" s="18">
         <v>1.5</v>
@@ -1190,21 +1486,24 @@
         <v>30</v>
       </c>
       <c r="E17" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s" s="18">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s" s="20">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s" s="20">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C18" s="20">
         <v>1.5</v>
@@ -1213,21 +1512,24 @@
         <v>30</v>
       </c>
       <c r="E18" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F18" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s" s="20">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s" s="20">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s" s="18">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C19" s="18">
         <v>1.5</v>
@@ -1236,21 +1538,24 @@
         <v>30</v>
       </c>
       <c r="E19" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s" s="18">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s" s="20">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C20" s="20">
         <v>1.5</v>
@@ -1259,21 +1564,24 @@
         <v>30</v>
       </c>
       <c r="E20" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s" s="20">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C21" s="5">
         <v>3</v>
@@ -1282,21 +1590,24 @@
         <v>75</v>
       </c>
       <c r="E21" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s" s="20">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s" s="20">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C22" s="20">
         <v>1</v>
@@ -1305,21 +1616,24 @@
         <v>25</v>
       </c>
       <c r="E22" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s" s="20">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="H22" t="s" s="20">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s" s="5">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C23" s="5">
         <v>1.5</v>
@@ -1328,21 +1642,24 @@
         <v>50</v>
       </c>
       <c r="E23" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s" s="3">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C24" s="3">
         <v>3</v>
@@ -1351,21 +1668,24 @@
         <v>75</v>
       </c>
       <c r="E24" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s" s="3">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s" s="18">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C25" s="18">
         <v>3</v>
@@ -1374,21 +1694,24 @@
         <v>75</v>
       </c>
       <c r="E25" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s" s="18">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s" s="20">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C26" s="20">
         <v>3</v>
@@ -1397,21 +1720,24 @@
         <v>75</v>
       </c>
       <c r="E26" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s" s="20">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s" s="18">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C27" s="18">
         <v>3</v>
@@ -1420,21 +1746,24 @@
         <v>75</v>
       </c>
       <c r="E27" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F27" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s" s="18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s" s="20">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C28" s="20">
         <v>3</v>
@@ -1443,21 +1772,24 @@
         <v>75</v>
       </c>
       <c r="E28" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s" s="20">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s" s="18">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C29" s="18">
         <v>3</v>
@@ -1466,21 +1798,24 @@
         <v>75</v>
       </c>
       <c r="E29" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s" s="18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s" s="20">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C30" s="20">
         <v>3</v>
@@ -1489,21 +1824,24 @@
         <v>75</v>
       </c>
       <c r="E30" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F30" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s" s="20">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s" s="18">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C31" s="18">
         <v>3</v>
@@ -1512,21 +1850,24 @@
         <v>75</v>
       </c>
       <c r="E31" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s" s="18">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s" s="20">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C32" s="20">
         <v>3</v>
@@ -1535,21 +1876,24 @@
         <v>75</v>
       </c>
       <c r="E32" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s" s="20">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s" s="18">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C33" s="18">
         <v>3</v>
@@ -1558,21 +1902,24 @@
         <v>75</v>
       </c>
       <c r="E33" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F33" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s" s="18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s" s="20">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C34" s="20">
         <v>3</v>
@@ -1581,21 +1928,24 @@
         <v>75</v>
       </c>
       <c r="E34" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F34" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s" s="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s" s="18">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C35" s="18">
         <v>3</v>
@@ -1604,21 +1954,24 @@
         <v>75</v>
       </c>
       <c r="E35" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F35" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s" s="18">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s" s="20">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C36" s="20">
         <v>3</v>
@@ -1627,21 +1980,24 @@
         <v>75</v>
       </c>
       <c r="E36" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F36" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s" s="20">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s" s="18">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C37" s="18">
         <v>3</v>
@@ -1650,21 +2006,24 @@
         <v>75</v>
       </c>
       <c r="E37" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F37" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s" s="18">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s" s="20">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C38" s="20">
         <v>3</v>
@@ -1673,21 +2032,24 @@
         <v>75</v>
       </c>
       <c r="E38" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F38" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H38" t="s" s="20">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s" s="18">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C39" s="18">
         <v>3</v>
@@ -1696,21 +2058,24 @@
         <v>75</v>
       </c>
       <c r="E39" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F39" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s" s="18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s" s="20">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C40" s="20">
         <v>3</v>
@@ -1719,21 +2084,24 @@
         <v>0</v>
       </c>
       <c r="E40" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H40" t="s" s="20">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s" s="18">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C41" s="18">
         <v>3</v>
@@ -1742,21 +2110,24 @@
         <v>0</v>
       </c>
       <c r="E41" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F41" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s" s="18">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s" s="3">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C42" s="3">
         <v>3</v>
@@ -1765,21 +2136,24 @@
         <v>0</v>
       </c>
       <c r="E42" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F42" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H42" t="s" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B43" t="s" s="18">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C43" s="18">
         <v>3</v>
@@ -1788,21 +2162,24 @@
         <v>0</v>
       </c>
       <c r="E43" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F43" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H43" t="s" s="18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s" s="20">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C44" s="20">
         <v>3</v>
@@ -1811,21 +2188,24 @@
         <v>0</v>
       </c>
       <c r="E44" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F44" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G44" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H44" t="s" s="20">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s" s="18">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C45" s="18">
         <v>3</v>
@@ -1834,21 +2214,24 @@
         <v>0</v>
       </c>
       <c r="E45" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F45" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s" s="18">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s" s="20">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="C46" s="20">
         <v>1</v>
@@ -1857,21 +2240,24 @@
         <v>0</v>
       </c>
       <c r="E46" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F46" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s" s="20">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s" s="18">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="C47" s="18">
         <v>1</v>
@@ -1880,21 +2266,24 @@
         <v>0</v>
       </c>
       <c r="E47" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F47" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s" s="18">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s" s="20">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="C48" s="20">
         <v>1</v>
@@ -1903,21 +2292,24 @@
         <v>0</v>
       </c>
       <c r="E48" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F48" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H48" t="s" s="20">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s" s="18">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="C49" s="18">
         <v>1</v>
@@ -1926,21 +2318,24 @@
         <v>0</v>
       </c>
       <c r="E49" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F49" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G49" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s" s="18">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s" s="20">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="C50" s="20">
         <v>2</v>
@@ -1949,21 +2344,24 @@
         <v>0</v>
       </c>
       <c r="E50" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F50" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G50" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s" s="20">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s" s="5">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s" s="5">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="C51" s="5">
         <v>0</v>
@@ -1972,21 +2370,24 @@
         <v>600</v>
       </c>
       <c r="E51" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F51" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G51" t="s" s="5">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" ht="25" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="H51" t="s" s="5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" ht="25" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s" s="3">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="C52" s="3">
         <v>3</v>
@@ -1995,21 +2396,24 @@
         <v>125</v>
       </c>
       <c r="E52" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F52" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H52" t="s" s="3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s" s="5">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="C53" s="5">
         <v>3</v>
@@ -2018,21 +2422,24 @@
         <v>75</v>
       </c>
       <c r="E53" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F53" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H53" t="s" s="5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s" s="20">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s" s="20">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C54" s="20">
         <v>1.5</v>
@@ -2041,21 +2448,24 @@
         <v>0</v>
       </c>
       <c r="E54" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F54" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s" s="20">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="H54" t="s" s="20">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s" s="18">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s" s="18">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C55" s="18">
         <v>1.5</v>
@@ -2064,21 +2474,24 @@
         <v>0</v>
       </c>
       <c r="E55" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F55" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s" s="18">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="H55" t="s" s="18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s" s="20">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="C56" s="20">
         <v>1.5</v>
@@ -2087,21 +2500,24 @@
         <v>0</v>
       </c>
       <c r="E56" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F56" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G56" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H56" t="s" s="20">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" ht="25" customHeight="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s" s="5">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s" s="5">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="C57" s="5">
         <v>0</v>
@@ -2110,21 +2526,24 @@
         <v>40</v>
       </c>
       <c r="E57" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F57" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G57" t="s" s="5">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="H57" t="s" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s" s="20">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s" s="20">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="C58" s="20">
         <v>1</v>
@@ -2133,21 +2552,24 @@
         <v>0</v>
       </c>
       <c r="E58" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F58" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G58" t="s" s="20">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="H58" t="s" s="20">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s" s="18">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="C59" s="18">
         <v>1</v>
@@ -2156,21 +2578,24 @@
         <v>0</v>
       </c>
       <c r="E59" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F59" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G59" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s" s="18">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s" s="20">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="B60" t="s" s="20">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C60" s="20">
         <v>2</v>
@@ -2179,21 +2604,24 @@
         <v>0</v>
       </c>
       <c r="E60" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F60" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G60" t="s" s="20">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="61" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="H60" t="s" s="20">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s" s="18">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s" s="18">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C61" s="18">
         <v>2</v>
@@ -2202,21 +2630,24 @@
         <v>0</v>
       </c>
       <c r="E61" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F61" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G61" t="s" s="18">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="H61" t="s" s="18">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s" s="20">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C62" s="20">
         <v>2</v>
@@ -2225,21 +2656,24 @@
         <v>0</v>
       </c>
       <c r="E62" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F62" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G62" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H62" t="s" s="20">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B63" t="s" s="18">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C63" s="18">
         <v>2</v>
@@ -2248,21 +2682,24 @@
         <v>0</v>
       </c>
       <c r="E63" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F63" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G63" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H63" t="s" s="18">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s" s="20">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C64" s="20">
         <v>2</v>
@@ -2271,21 +2708,24 @@
         <v>0</v>
       </c>
       <c r="E64" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F64" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G64" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H64" t="s" s="20">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s" s="18">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C65" s="18">
         <v>2</v>
@@ -2294,21 +2734,24 @@
         <v>0</v>
       </c>
       <c r="E65" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F65" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G65" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H65" t="s" s="18">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B66" t="s" s="20">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C66" s="20">
         <v>2</v>
@@ -2317,21 +2760,24 @@
         <v>0</v>
       </c>
       <c r="E66" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F66" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G66" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H66" t="s" s="20">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s" s="18">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C67" s="18">
         <v>2</v>
@@ -2340,21 +2786,24 @@
         <v>0</v>
       </c>
       <c r="E67" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F67" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G67" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H67" t="s" s="18">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B68" t="s" s="20">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C68" s="20">
         <v>2</v>
@@ -2363,21 +2812,24 @@
         <v>0</v>
       </c>
       <c r="E68" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F68" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G68" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H68" t="s" s="20">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B69" t="s" s="18">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="C69" s="18">
         <v>2</v>
@@ -2386,21 +2838,24 @@
         <v>0</v>
       </c>
       <c r="E69" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F69" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G69" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H69" t="s" s="18">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s" s="20">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B70" t="s" s="20">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C70" s="20">
         <v>2</v>
@@ -2409,21 +2864,24 @@
         <v>0</v>
       </c>
       <c r="E70" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F70" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" t="s" s="20">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="71" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="H70" t="s" s="20">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="71" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B71" t="s" s="18">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C71" s="18">
         <v>2</v>
@@ -2432,21 +2890,24 @@
         <v>0</v>
       </c>
       <c r="E71" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F71" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G71" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H71" t="s" s="18">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s" s="20">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C72" s="20">
         <v>2</v>
@@ -2455,21 +2916,24 @@
         <v>0</v>
       </c>
       <c r="E72" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F72" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G72" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H72" t="s" s="20">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s" s="18">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C73" s="18">
         <v>2</v>
@@ -2478,21 +2942,24 @@
         <v>0</v>
       </c>
       <c r="E73" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F73" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G73" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H73" t="s" s="18">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B74" t="s" s="20">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C74" s="20">
         <v>2</v>
@@ -2501,21 +2968,24 @@
         <v>0</v>
       </c>
       <c r="E74" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F74" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G74" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H74" t="s" s="20">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s" s="18">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C75" s="18">
         <v>2</v>
@@ -2524,21 +2994,24 @@
         <v>0</v>
       </c>
       <c r="E75" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F75" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G75" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H75" t="s" s="18">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s" s="20">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C76" s="20">
         <v>2</v>
@@ -2547,21 +3020,24 @@
         <v>0</v>
       </c>
       <c r="E76" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F76" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G76" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H76" t="s" s="20">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s" s="18">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C77" s="18">
         <v>2</v>
@@ -2570,21 +3046,24 @@
         <v>0</v>
       </c>
       <c r="E77" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F77" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G77" t="s" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" ht="25" customHeight="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H77" t="s" s="18">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" ht="25" customHeight="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B78" t="s" s="20">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C78" s="20">
         <v>2</v>
@@ -2593,21 +3072,24 @@
         <v>0</v>
       </c>
       <c r="E78" t="s" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F78" t="s" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G78" t="s" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" ht="25" customHeight="1" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H78" t="s" s="20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" ht="25" customHeight="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B79" t="s" s="18">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="C79" s="18">
         <v>2</v>
@@ -2616,13 +3098,21 @@
         <v>0</v>
       </c>
       <c r="E79" t="s" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F79" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G79" t="s" s="18">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H79" t="s" s="18">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>